<commit_message>
fixed trial D in runs log
</commit_message>
<xml_diff>
--- a/Drone_Runs_log.xlsx
+++ b/Drone_Runs_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timkj\OneDrive\Documents\GitHub\Wildfire_Drone_SJSU_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4861C0-2C84-4987-8E8C-4C14DA6F9060}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9213C945-91F7-421D-A117-C002BA7BCDE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C0B6D431-78E4-472A-8865-D34C597A569E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>trial</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>mountain in full view, crashed. Depth can't distinguish.</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -285,68 +288,68 @@
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,28 +674,28 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="50" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -709,363 +712,398 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="2" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="20" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="20.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="2" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="20" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>3</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>4</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>5</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="11" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="11" t="s">
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="11" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="L9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="M9" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="13"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="11" t="s">
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="M12" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="13"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D6:D8"/>
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="M12:M14"/>
     <mergeCell ref="M9:M11"/>
@@ -1081,42 +1119,7 @@
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
     <mergeCell ref="L9:L11"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="M6:M8"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="H3:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>